<commit_message>
#3 Correct Excel spreadsheets
</commit_message>
<xml_diff>
--- a/Excel/Manufacturing optimisation exercise.xlsx
+++ b/Excel/Manufacturing optimisation exercise.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Team Quantum Programme\Quantum data Centre of the future\30. Technology Access Programme Design\Training material\15 Optimisations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielGoldsmith\Desktop\Python workbooks\QTAP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A3E626-EB9C-46CD-9EF1-753050796172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DD4F20-7995-4DD2-B89B-01DD0D56FA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2215,23 +2215,23 @@
       </c>
       <c r="J4" s="8">
         <f>B13*B4</f>
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="8">
         <f t="shared" ref="K4:M6" si="0">C13*C$8</f>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="L4" s="8">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="8">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="21">
         <f>J4-K4-L4-M4</f>
-        <v>29200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -2257,23 +2257,23 @@
       </c>
       <c r="J5" s="8">
         <f>B14*B5</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="K5" s="8">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="L5" s="8">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="M5" s="8">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="N5" s="21">
         <f>J5-K5-L5-M5</f>
-        <v>79000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2299,23 +2299,23 @@
       </c>
       <c r="J6" s="16">
         <f>B15*B6</f>
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="K6" s="16">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="L6" s="16">
         <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="M6" s="16">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="N6" s="22">
         <f>J6-K6-L6-M6</f>
-        <v>22600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="J9" s="5">
         <f>SUM(N4:N6)</f>
-        <v>130800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -2404,19 +2404,19 @@
         <v>0</v>
       </c>
       <c r="B13" s="27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C13" s="9">
         <f t="shared" ref="C13:E15" si="1">$B13*C4</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2424,19 +2424,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="27">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C14" s="9">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2446,19 +2446,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C15" s="9">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -2470,15 +2470,15 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9">
         <f>SUM(C13:C15)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" ref="D16:E16" si="2">SUM(D13:D15)</f>
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="2"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>

</xml_diff>

<commit_message>
#3 Correct Excel spreadsheets (#5)
</commit_message>
<xml_diff>
--- a/Excel/Manufacturing optimisation exercise.xlsx
+++ b/Excel/Manufacturing optimisation exercise.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Team Quantum Programme\Quantum data Centre of the future\30. Technology Access Programme Design\Training material\15 Optimisations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielGoldsmith\Desktop\Python workbooks\QTAP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A3E626-EB9C-46CD-9EF1-753050796172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DD4F20-7995-4DD2-B89B-01DD0D56FA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2215,23 +2215,23 @@
       </c>
       <c r="J4" s="8">
         <f>B13*B4</f>
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="8">
         <f t="shared" ref="K4:M6" si="0">C13*C$8</f>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="L4" s="8">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="8">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="21">
         <f>J4-K4-L4-M4</f>
-        <v>29200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -2257,23 +2257,23 @@
       </c>
       <c r="J5" s="8">
         <f>B14*B5</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="K5" s="8">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="L5" s="8">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="M5" s="8">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="N5" s="21">
         <f>J5-K5-L5-M5</f>
-        <v>79000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2299,23 +2299,23 @@
       </c>
       <c r="J6" s="16">
         <f>B15*B6</f>
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="K6" s="16">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="L6" s="16">
         <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="M6" s="16">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="N6" s="22">
         <f>J6-K6-L6-M6</f>
-        <v>22600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="J9" s="5">
         <f>SUM(N4:N6)</f>
-        <v>130800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -2404,19 +2404,19 @@
         <v>0</v>
       </c>
       <c r="B13" s="27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C13" s="9">
         <f t="shared" ref="C13:E15" si="1">$B13*C4</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2424,19 +2424,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="27">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C14" s="9">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2446,19 +2446,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C15" s="9">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -2470,15 +2470,15 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9">
         <f>SUM(C13:C15)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" ref="D16:E16" si="2">SUM(D13:D15)</f>
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="2"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>

</xml_diff>